<commit_message>
Upaded Box for single eye detection
</commit_message>
<xml_diff>
--- a/Code/CroppedSetMaskorNot.xlsx
+++ b/Code/CroppedSetMaskorNot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli Clark\Documents\Fall_20\ELE_400\FinalProject\ELE400_FinalProject\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316BC520-C80D-41B9-8448-8A7117E67252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57B60D6-8B3A-4F21-8ADB-10040EC0A3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1098" yWindow="570" windowWidth="17280" windowHeight="8994" xr2:uid="{CAC5F023-D520-4236-85AB-C3C3B9BC574C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>'0001.jpg'</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>H_ext = 2.5</t>
+  </si>
+  <si>
+    <t>Swapped Ifelse order H_ext = 2</t>
   </si>
 </sst>
 </file>
@@ -701,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C0636C-151C-4EB3-8FE2-CE8DB045187F}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -713,9 +716,10 @@
     <col min="2" max="2" width="11.05078125" customWidth="1"/>
     <col min="3" max="3" width="11.1015625" customWidth="1"/>
     <col min="5" max="5" width="9.9453125" customWidth="1"/>
+    <col min="6" max="6" width="25.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -731,8 +735,11 @@
       <c r="E1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -748,8 +755,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -757,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -765,8 +775,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -774,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -782,8 +795,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -799,8 +815,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -808,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -816,8 +835,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -833,8 +855,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -850,8 +875,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -867,8 +895,11 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -884,8 +915,11 @@
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -901,8 +935,11 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -918,8 +955,11 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -935,8 +975,11 @@
       <c r="E13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -952,8 +995,11 @@
       <c r="E14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -961,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -969,8 +1015,11 @@
       <c r="E15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -978,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -986,8 +1035,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1003,8 +1055,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1020,8 +1075,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1037,8 +1095,11 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1046,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1054,8 +1115,11 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1071,8 +1135,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1088,8 +1155,11 @@
       <c r="E22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1105,8 +1175,11 @@
       <c r="E23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1122,8 +1195,11 @@
       <c r="E24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1131,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1139,8 +1215,11 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1148,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1156,8 +1235,11 @@
       <c r="E26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1173,8 +1255,11 @@
       <c r="E27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1182,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1190,8 +1275,11 @@
       <c r="E28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1199,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1207,8 +1295,11 @@
       <c r="E29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1216,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1224,8 +1315,11 @@
       <c r="E30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1241,8 +1335,11 @@
       <c r="E31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1258,8 +1355,11 @@
       <c r="E32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1267,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1275,8 +1375,11 @@
       <c r="E33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1292,8 +1395,11 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1309,8 +1415,11 @@
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1326,8 +1435,11 @@
       <c r="E36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1335,7 +1447,7 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1343,8 +1455,11 @@
       <c r="E37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1360,8 +1475,11 @@
       <c r="E38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1377,8 +1495,11 @@
       <c r="E39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1394,8 +1515,11 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1403,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1411,8 +1535,11 @@
       <c r="E41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1420,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1428,8 +1555,11 @@
       <c r="E42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1445,8 +1575,11 @@
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1462,8 +1595,11 @@
       <c r="E44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1471,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1479,8 +1615,11 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1496,8 +1635,11 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1513,8 +1655,11 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1530,8 +1675,11 @@
       <c r="E48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1539,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1547,8 +1695,11 @@
       <c r="E49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1556,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1564,8 +1715,11 @@
       <c r="E50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1573,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1581,8 +1735,11 @@
       <c r="E51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1590,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1598,8 +1755,11 @@
       <c r="E52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1615,8 +1775,11 @@
       <c r="E53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1624,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -1632,8 +1795,11 @@
       <c r="E54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1641,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -1649,8 +1815,11 @@
       <c r="E55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1666,8 +1835,11 @@
       <c r="E56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1675,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -1683,8 +1855,11 @@
       <c r="E57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1692,7 +1867,7 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -1700,8 +1875,11 @@
       <c r="E58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1717,8 +1895,11 @@
       <c r="E59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1726,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -1734,8 +1915,11 @@
       <c r="E60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1751,8 +1935,11 @@
       <c r="E61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1768,8 +1955,11 @@
       <c r="E62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1777,7 +1967,7 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -1785,8 +1975,11 @@
       <c r="E63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1794,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -1802,8 +1995,11 @@
       <c r="E64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1811,7 +2007,7 @@
         <v>0</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -1819,8 +2015,11 @@
       <c r="E65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1828,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -1836,8 +2035,11 @@
       <c r="E66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -1853,8 +2055,11 @@
       <c r="E67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -1870,8 +2075,11 @@
       <c r="E68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -1879,7 +2087,7 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -1887,8 +2095,11 @@
       <c r="E69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -1896,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -1904,8 +2115,11 @@
       <c r="E70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -1913,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -1921,8 +2135,11 @@
       <c r="E71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -1930,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -1938,8 +2155,11 @@
       <c r="E72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -1947,7 +2167,7 @@
         <v>1</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -1955,8 +2175,11 @@
       <c r="E73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -1972,8 +2195,11 @@
       <c r="E74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -1989,8 +2215,11 @@
       <c r="E75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -1998,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -2006,8 +2235,11 @@
       <c r="E76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2015,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2023,8 +2255,11 @@
       <c r="E77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2032,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -2040,8 +2275,11 @@
       <c r="E78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2057,8 +2295,11 @@
       <c r="E79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2066,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -2074,8 +2315,11 @@
       <c r="E80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2083,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2091,8 +2335,11 @@
       <c r="E81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2108,8 +2355,11 @@
       <c r="E82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -2117,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -2125,8 +2375,11 @@
       <c r="E83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -2134,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -2142,8 +2395,11 @@
       <c r="E84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -2159,8 +2415,11 @@
       <c r="E85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -2168,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -2176,8 +2435,11 @@
       <c r="E86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -2193,8 +2455,11 @@
       <c r="E87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -2202,7 +2467,7 @@
         <v>1</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -2210,8 +2475,11 @@
       <c r="E88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -2219,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -2227,8 +2495,11 @@
       <c r="E89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -2244,8 +2515,11 @@
       <c r="E90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -2261,8 +2535,11 @@
       <c r="E91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -2270,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -2278,8 +2555,11 @@
       <c r="E92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -2295,8 +2575,11 @@
       <c r="E93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -2312,8 +2595,11 @@
       <c r="E94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -2329,8 +2615,11 @@
       <c r="E95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -2346,8 +2635,11 @@
       <c r="E96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -2363,8 +2655,11 @@
       <c r="E97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -2372,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -2380,8 +2675,11 @@
       <c r="E98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -2397,8 +2695,11 @@
       <c r="E99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -2406,7 +2707,7 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -2414,8 +2715,11 @@
       <c r="E100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
         <v>101</v>
       </c>
@@ -2423,16 +2727,20 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D101">
         <v>0</v>
       </c>
       <c r="E101">
         <v>0</v>
+      </c>
+      <c r="F101" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Playing With mean and median colors
</commit_message>
<xml_diff>
--- a/Code/CroppedSetMaskorNot.xlsx
+++ b/Code/CroppedSetMaskorNot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli Clark\Documents\Fall_20\ELE_400\FinalProject\ELE400_FinalProject\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57B60D6-8B3A-4F21-8ADB-10040EC0A3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2F6107-93AA-4D91-B383-4FFC36A209AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1098" yWindow="570" windowWidth="17280" windowHeight="8994" xr2:uid="{CAC5F023-D520-4236-85AB-C3C3B9BC574C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>'0001.jpg'</t>
   </si>
@@ -340,18 +340,6 @@
   </si>
   <si>
     <t>0412.jpg'</t>
-  </si>
-  <si>
-    <t>H_ext = 1.5</t>
-  </si>
-  <si>
-    <t>H_ext = 2</t>
-  </si>
-  <si>
-    <t>H_ext = 2.5</t>
-  </si>
-  <si>
-    <t>Swapped Ifelse order H_ext = 2</t>
   </si>
 </sst>
 </file>
@@ -704,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C0636C-151C-4EB3-8FE2-CE8DB045187F}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -719,27 +707,15 @@
     <col min="6" max="6" width="25.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -749,17 +725,8 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -767,19 +734,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -789,17 +747,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -809,17 +758,8 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -829,17 +769,8 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -849,17 +780,8 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -869,17 +791,8 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -889,17 +802,8 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -909,17 +813,8 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -929,17 +824,8 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -949,17 +835,8 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -969,17 +846,8 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -989,17 +857,8 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1007,19 +866,10 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1029,17 +879,8 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1049,17 +890,8 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1069,17 +901,8 @@
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1089,17 +912,8 @@
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1109,17 +923,8 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1129,17 +934,8 @@
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1149,17 +945,8 @@
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1169,17 +956,8 @@
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1189,17 +967,8 @@
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1209,17 +978,8 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1229,17 +989,8 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1249,17 +1000,8 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1269,17 +1011,8 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1289,17 +1022,8 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1309,17 +1033,8 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1329,17 +1044,8 @@
       <c r="C31">
         <v>0</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1349,17 +1055,8 @@
       <c r="C32">
         <v>0</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1369,17 +1066,8 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1389,17 +1077,8 @@
       <c r="C34">
         <v>0</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1409,17 +1088,8 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1429,17 +1099,8 @@
       <c r="C36">
         <v>0</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1449,17 +1110,8 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1469,17 +1121,8 @@
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1489,17 +1132,8 @@
       <c r="C39">
         <v>0</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1509,17 +1143,8 @@
       <c r="C40">
         <v>0</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1529,17 +1154,8 @@
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1549,17 +1165,8 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1569,17 +1176,8 @@
       <c r="C43">
         <v>0</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1589,17 +1187,8 @@
       <c r="C44">
         <v>0</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1609,17 +1198,8 @@
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1629,17 +1209,8 @@
       <c r="C46">
         <v>0</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1649,17 +1220,8 @@
       <c r="C47">
         <v>0</v>
       </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1669,17 +1231,8 @@
       <c r="C48">
         <v>0</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1687,19 +1240,10 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1707,19 +1251,10 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1727,19 +1262,10 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1747,19 +1273,10 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1769,17 +1286,8 @@
       <c r="C53">
         <v>0</v>
       </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1789,17 +1297,8 @@
       <c r="C54">
         <v>1</v>
       </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1807,19 +1306,10 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1829,17 +1319,8 @@
       <c r="C56">
         <v>0</v>
       </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1849,17 +1330,8 @@
       <c r="C57">
         <v>1</v>
       </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1869,17 +1341,8 @@
       <c r="C58">
         <v>1</v>
       </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1889,17 +1352,8 @@
       <c r="C59">
         <v>1</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1907,19 +1361,10 @@
         <v>1</v>
       </c>
       <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1929,17 +1374,8 @@
       <c r="C61">
         <v>0</v>
       </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1949,17 +1385,8 @@
       <c r="C62">
         <v>1</v>
       </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1967,19 +1394,10 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1989,17 +1407,8 @@
       <c r="C64">
         <v>1</v>
       </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2007,19 +1416,10 @@
         <v>0</v>
       </c>
       <c r="C65">
-        <v>1</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2029,17 +1429,8 @@
       <c r="C66">
         <v>1</v>
       </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2049,17 +1440,8 @@
       <c r="C67">
         <v>0</v>
       </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2069,17 +1451,8 @@
       <c r="C68">
         <v>0</v>
       </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2089,17 +1462,8 @@
       <c r="C69">
         <v>1</v>
       </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2109,17 +1473,8 @@
       <c r="C70">
         <v>1</v>
       </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2129,17 +1484,8 @@
       <c r="C71">
         <v>1</v>
       </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2149,17 +1495,8 @@
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="F72" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2169,17 +1506,8 @@
       <c r="C73">
         <v>1</v>
       </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2189,17 +1517,8 @@
       <c r="C74">
         <v>0</v>
       </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2209,17 +1528,8 @@
       <c r="C75">
         <v>0</v>
       </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2227,19 +1537,10 @@
         <v>1</v>
       </c>
       <c r="C76">
-        <v>1</v>
-      </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2249,17 +1550,8 @@
       <c r="C77">
         <v>1</v>
       </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2267,19 +1559,10 @@
         <v>1</v>
       </c>
       <c r="C78">
-        <v>1</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2289,17 +1572,8 @@
       <c r="C79">
         <v>0</v>
       </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2309,17 +1583,8 @@
       <c r="C80">
         <v>1</v>
       </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2329,17 +1594,8 @@
       <c r="C81">
         <v>1</v>
       </c>
-      <c r="D81">
-        <v>0</v>
-      </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
-      <c r="F81" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2349,17 +1605,8 @@
       <c r="C82">
         <v>0</v>
       </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-      <c r="F82" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -2369,17 +1616,8 @@
       <c r="C83">
         <v>1</v>
       </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="F83" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -2389,17 +1627,8 @@
       <c r="C84">
         <v>1</v>
       </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-      <c r="F84" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -2409,17 +1638,8 @@
       <c r="C85">
         <v>0</v>
       </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-      <c r="F85" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -2429,17 +1649,8 @@
       <c r="C86">
         <v>1</v>
       </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86">
-        <v>0</v>
-      </c>
-      <c r="F86" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -2449,17 +1660,8 @@
       <c r="C87">
         <v>0</v>
       </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-      <c r="E87">
-        <v>0</v>
-      </c>
-      <c r="F87" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -2467,19 +1669,10 @@
         <v>1</v>
       </c>
       <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
-      <c r="E88">
-        <v>0</v>
-      </c>
-      <c r="F88" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -2489,17 +1682,8 @@
       <c r="C89">
         <v>1</v>
       </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
-      <c r="E89">
-        <v>0</v>
-      </c>
-      <c r="F89" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -2509,17 +1693,8 @@
       <c r="C90">
         <v>0</v>
       </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
-      <c r="E90">
-        <v>0</v>
-      </c>
-      <c r="F90" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -2529,17 +1704,8 @@
       <c r="C91">
         <v>0</v>
       </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-      <c r="F91" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -2549,17 +1715,8 @@
       <c r="C92">
         <v>1</v>
       </c>
-      <c r="D92">
-        <v>0</v>
-      </c>
-      <c r="E92">
-        <v>0</v>
-      </c>
-      <c r="F92" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -2569,17 +1726,8 @@
       <c r="C93">
         <v>1</v>
       </c>
-      <c r="D93">
-        <v>1</v>
-      </c>
-      <c r="E93">
-        <v>1</v>
-      </c>
-      <c r="F93" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -2589,17 +1737,8 @@
       <c r="C94">
         <v>0</v>
       </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -2609,17 +1748,8 @@
       <c r="C95">
         <v>1</v>
       </c>
-      <c r="D95">
-        <v>1</v>
-      </c>
-      <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -2629,17 +1759,8 @@
       <c r="C96">
         <v>1</v>
       </c>
-      <c r="D96">
-        <v>1</v>
-      </c>
-      <c r="E96">
-        <v>1</v>
-      </c>
-      <c r="F96" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -2649,17 +1770,8 @@
       <c r="C97">
         <v>0</v>
       </c>
-      <c r="D97">
-        <v>0</v>
-      </c>
-      <c r="E97">
-        <v>0</v>
-      </c>
-      <c r="F97" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -2669,17 +1781,8 @@
       <c r="C98">
         <v>1</v>
       </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
-      <c r="E98">
-        <v>0</v>
-      </c>
-      <c r="F98" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -2689,17 +1792,8 @@
       <c r="C99">
         <v>1</v>
       </c>
-      <c r="D99">
-        <v>1</v>
-      </c>
-      <c r="E99">
-        <v>1</v>
-      </c>
-      <c r="F99" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -2707,19 +1801,10 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <v>1</v>
-      </c>
-      <c r="D100">
-        <v>0</v>
-      </c>
-      <c r="E100">
-        <v>0</v>
-      </c>
-      <c r="F100" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
         <v>101</v>
       </c>
@@ -2727,15 +1812,6 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>1</v>
-      </c>
-      <c r="D101">
-        <v>0</v>
-      </c>
-      <c r="E101">
-        <v>0</v>
-      </c>
-      <c r="F101" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>